<commit_message>
All of Tays new cool stuff
</commit_message>
<xml_diff>
--- a/shinyapp/data/Sterling_Youth_Development.xlsx
+++ b/shinyapp/data/Sterling_Youth_Development.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Downloads/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6AA32FE-84A9-094C-82D4-7444E38124D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BB54EA-9131-C646-A0FB-1F1262F68971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -595,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08265865-87B3-A141-B92B-A5F35EC84153}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="G12" sqref="G12:G19"/>
     </sheetView>
   </sheetViews>

</xml_diff>